<commit_message>
Changed gitignore and experimented with vaadin scrum first sprint defined
</commit_message>
<xml_diff>
--- a/doc/scrum_green.xlsx
+++ b/doc/scrum_green.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="120" windowWidth="22760" windowHeight="11920"/>
+    <workbookView xWindow="380" yWindow="120" windowWidth="28960" windowHeight="17640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -52,21 +52,6 @@
     <t>work in progress</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>cancelled</t>
-  </si>
-  <si>
-    <t>100h</t>
-  </si>
-  <si>
-    <t>200h</t>
-  </si>
-  <si>
-    <t>400h</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -82,21 +67,6 @@
     <t>Effort Actual</t>
   </si>
   <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Hans</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
     <t>UI, Controller</t>
   </si>
   <si>
@@ -106,12 +76,6 @@
     <t>Main Window</t>
   </si>
   <si>
-    <t>Patient Model</t>
-  </si>
-  <si>
-    <t>Data model for patient record needs to be created based on standard....</t>
-  </si>
-  <si>
     <t>Effort Plan Original</t>
   </si>
   <si>
@@ -127,26 +91,192 @@
     <t>Skills</t>
   </si>
   <si>
-    <t>Settings</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ein Reminder erinnert Patient an Medikamenteinnahme zur richtigen Zeit und in der korrekten Dosis </t>
   </si>
   <si>
     <t xml:space="preserve">Erinnert den Benutzer der App an die Einnahme von Medikamenten, welche vom Arzt in die Liste der einzunehmenden Medikamente eingefügt wurde. Die Medikamente werden mit der empfohlenen Dosis eingetragen und dem Patienten für die Einnahme mit Anzeige der empfohlenen Dosis angezeigt. </t>
   </si>
   <si>
-    <t>Setting up different Configurations for the other Modules</t>
-  </si>
-  <si>
     <t>Der Patient kann seine definierten Skills -Funktion aufrufen</t>
+  </si>
+  <si>
+    <t>Package Diagram</t>
+  </si>
+  <si>
+    <t>System Architecture</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">design a software architecture taking into account
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Orator Std Slanted"/>
+        <family val="2"/>
+      </rPr>
+      <t>▶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> system requirements
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Orator Std Slanted"/>
+        <family val="2"/>
+      </rPr>
+      <t>▶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> incl. the need for persistent data storage
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Orator Std Slanted"/>
+        <family val="2"/>
+      </rPr>
+      <t>▶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> architectural design patterns
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Orator Std Slanted"/>
+        <family val="2"/>
+      </rPr>
+      <t>▶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the Vaadin framework</t>
+    </r>
+  </si>
+  <si>
+    <t>Creating a UML package diagram to show the high-level structure of application.</t>
+  </si>
+  <si>
+    <t>gnagj1</t>
+  </si>
+  <si>
+    <t>vonkc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mainview </t>
+  </si>
+  <si>
+    <t>Helpview</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Create a Model based on the Requirements for the Help Scenario</t>
+  </si>
+  <si>
+    <t>Class Diagramm</t>
+  </si>
+  <si>
+    <t>LoginView</t>
+  </si>
+  <si>
+    <t>Create a Login view for later user specific Data Handling</t>
+  </si>
+  <si>
+    <t>BLL</t>
+  </si>
+  <si>
+    <t>User Data Manager</t>
+  </si>
+  <si>
+    <t>Create a Manager that gets the right Data based on the View and the logged in user</t>
+  </si>
+  <si>
+    <t>LoginManager</t>
+  </si>
+  <si>
+    <t>Based on the Login Data given the Manager must grant access or dissalow by checking data from database</t>
+  </si>
+  <si>
+    <t>Create a Class Diagram / Domain Diagram for classes required</t>
+  </si>
+  <si>
+    <t>Create the Helpview with its Controller and also beginn with the corresponding Settings view</t>
+  </si>
+  <si>
+    <t>Create the Mainview of the Application in which the different views are displayed and a ViewManager</t>
+  </si>
+  <si>
+    <t>80h</t>
+  </si>
+  <si>
+    <t>70h</t>
+  </si>
+  <si>
+    <t>150h</t>
+  </si>
+  <si>
+    <t>MedicView</t>
+  </si>
+  <si>
+    <t>Create the MedicView with its Controller and also beginn with the corresponding Settings view</t>
+  </si>
+  <si>
+    <t>Persistent Storage</t>
+  </si>
+  <si>
+    <t>Store for the different Personal Data</t>
+  </si>
+  <si>
+    <t>SkillsView</t>
+  </si>
+  <si>
+    <t>Create the SkillsView with its Controller and also beginn with the corresponding Settings view</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +302,28 @@
       <color theme="1"/>
       <name val="TimesNewRomanPSMT"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Orator Std Slanted"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -196,25 +348,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -516,15 +699,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="46.1640625" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
@@ -532,67 +715,64 @@
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="14" customHeight="1">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -600,37 +780,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:H5">
@@ -648,24 +825,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.1640625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -674,95 +851,89 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="56">
+    <row r="2" spans="1:11" ht="78">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28">
       <c r="A3">
         <v>1.2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3">
-        <v>8</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
@@ -775,70 +946,66 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
       </c>
       <c r="H4">
-        <v>16</v>
-      </c>
-      <c r="I4">
-        <v>20</v>
-      </c>
-      <c r="J4">
-        <f>SUM(I4:I4)</f>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28">
       <c r="A5">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
         <v>10</v>
       </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
       <c r="K5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28">
       <c r="A6">
-        <v>2.2000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -846,18 +1013,207 @@
       <c r="H6">
         <v>8</v>
       </c>
-      <c r="I6">
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>1.6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
         <v>6</v>
       </c>
-      <c r="J6">
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>1.7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28">
+      <c r="A9">
+        <v>1.8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28">
+      <c r="A10">
+        <v>1.9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>19</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28">
+      <c r="A11">
+        <v>2.1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" t="s">
         <v>5</v>
       </c>
-      <c r="K6" t="s">
-        <v>9</v>
+    </row>
+    <row r="12" spans="1:11" ht="28">
+      <c r="A12">
+        <v>3.1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>2.4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>2.5</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>2.6</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2.7</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2.8</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2.9</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Data Generation and data handling in model and data access arranged
</commit_message>
<xml_diff>
--- a/doc/scrum_green.xlsx
+++ b/doc/scrum_green.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="0" windowWidth="26520" windowHeight="20480" activeTab="1"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="26520" windowHeight="20480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1313,27 +1313,18 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="B18">
-        <v>2</v>
-      </c>
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11">
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="B20">
-        <v>2</v>
-      </c>
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11">
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="B22">
-        <v>2</v>
-      </c>
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" s="8" customFormat="1">

</xml_diff>

<commit_message>
Updated Diary and Scrum-Planning
</commit_message>
<xml_diff>
--- a/doc/scrum_green.xlsx
+++ b/doc/scrum_green.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -112,12 +112,6 @@
     <t>Create a Login view for later user specific Data Handling</t>
   </si>
   <si>
-    <t>User Data Manager</t>
-  </si>
-  <si>
-    <t>Create a Manager that gets the right Data based on the View and the logged in user</t>
-  </si>
-  <si>
     <t>LoginManager</t>
   </si>
   <si>
@@ -230,6 +224,33 @@
   </si>
   <si>
     <t>UI, BLL</t>
+  </si>
+  <si>
+    <t>Styling</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Find a Part that is likely to change to implement State Pattern</t>
+  </si>
+  <si>
+    <t>Encryption of passwords</t>
+  </si>
+  <si>
+    <t>BLL, LoginManager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Data </t>
+  </si>
+  <si>
+    <t>User Data Manager, DataAccess</t>
+  </si>
+  <si>
+    <t>Implement logic to get specific Data for the logged in User</t>
   </si>
 </sst>
 </file>
@@ -314,8 +335,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -404,7 +431,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="69">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -436,6 +463,9 @@
     <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -467,6 +497,9 @@
     <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -824,10 +857,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -844,7 +877,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
@@ -864,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
         <v>8</v>
@@ -890,10 +923,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -902,7 +935,7 @@
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="31.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
     <col min="8" max="8" width="7.1640625" customWidth="1"/>
@@ -960,13 +993,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -974,8 +1007,11 @@
       <c r="H2">
         <v>10</v>
       </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
       <c r="K2" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28">
@@ -989,13 +1025,13 @@
         <v>27</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -1003,8 +1039,11 @@
       <c r="H3">
         <v>8</v>
       </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
       <c r="K3" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1015,16 +1054,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -1032,8 +1071,11 @@
       <c r="H4">
         <v>8</v>
       </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
       <c r="K4" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="42">
@@ -1044,16 +1086,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -1061,8 +1103,14 @@
       <c r="H5">
         <v>4</v>
       </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
       <c r="K5" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="28">
@@ -1079,7 +1127,7 @@
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -1090,8 +1138,14 @@
       <c r="H6">
         <v>6</v>
       </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
       <c r="K6" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="42">
@@ -1102,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -1119,48 +1173,15 @@
       <c r="H7">
         <v>19</v>
       </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
       <c r="K7" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="42">
-      <c r="A10">
-        <v>1.9</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10">
-        <v>19</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>8</v>
-      </c>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" s="8" customFormat="1">
       <c r="D11" s="9"/>
@@ -1173,19 +1194,22 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
       </c>
       <c r="H12">
         <v>10</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1196,19 +1220,22 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="28">
@@ -1219,22 +1246,31 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
         <v>25</v>
       </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
       <c r="H14">
         <v>10</v>
       </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
       <c r="K14" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1245,19 +1281,25 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
+      <c r="I15">
+        <v>12</v>
+      </c>
       <c r="K15" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1268,22 +1310,31 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
       </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
       <c r="H16">
         <v>8</v>
       </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
       <c r="K16" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1294,16 +1345,16 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
@@ -1312,17 +1363,133 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="K18" s="10"/>
+    <row r="18" spans="1:11" ht="42">
+      <c r="A18">
+        <v>1.4</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="K21" s="10"/>
+      <c r="A19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>6</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="28">
+      <c r="A20">
+        <v>2.7</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="28">
+      <c r="A21">
+        <v>2.8</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
       <c r="K22" s="10"/>
@@ -1334,17 +1501,14 @@
       <c r="A24">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
         <v>38</v>
-      </c>
-      <c r="E24" t="s">
-        <v>40</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
@@ -1360,17 +1524,14 @@
       <c r="A25">
         <v>4.2</v>
       </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
       <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
@@ -1386,14 +1547,11 @@
       <c r="A26">
         <v>4.3</v>
       </c>
-      <c r="B26">
-        <v>3</v>
-      </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
@@ -1406,6 +1564,11 @@
       </c>
       <c r="K26" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="C27" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last changes in scrum logs
</commit_message>
<xml_diff>
--- a/doc/scrum_green.xlsx
+++ b/doc/scrum_green.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="0" windowWidth="26520" windowHeight="20480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -220,9 +220,6 @@
     <t>UI</t>
   </si>
   <si>
-    <t>MedicationView Settings</t>
-  </si>
-  <si>
     <t>UI, BLL</t>
   </si>
   <si>
@@ -251,13 +248,16 @@
   </si>
   <si>
     <t>Implement logic to get specific Data for the logged in User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medication Settings View </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,8 +305,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +340,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0F243E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -335,7 +362,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -405,8 +432,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -417,21 +448,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="73">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -466,6 +503,8 @@
     <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -500,6 +539,8 @@
     <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -925,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -934,7 +975,7 @@
     <col min="1" max="1" width="6.1640625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="31.5" style="6" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
@@ -948,628 +989,743 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="42">
-      <c r="A2">
+      <c r="A2" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="10">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="10">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10">
         <v>4</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28">
-      <c r="A3">
+      <c r="A3" s="10">
         <v>1.2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="10">
         <v>8</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="10">
         <v>8</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="10"/>
+      <c r="K3" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4">
+      <c r="A4" s="10">
         <v>1.3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="10">
         <v>8</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="10">
         <v>10</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="J4" s="10"/>
+      <c r="K4" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="42">
-      <c r="A5">
+      <c r="A5" s="10">
         <v>1.4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="10">
         <v>4</v>
       </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5" s="10" t="s">
+      <c r="I5" s="10">
+        <v>2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>2</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="28">
-      <c r="A6">
+      <c r="A6" s="10">
         <v>1.5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="10">
         <v>6</v>
       </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="I6" s="10">
+        <v>2</v>
+      </c>
+      <c r="J6" s="10">
+        <v>2</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="42">
-      <c r="A7">
+      <c r="A7" s="10">
         <v>1.6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="10">
         <v>19</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="10">
         <v>10</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="J7" s="10">
+        <v>6</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" s="7" customFormat="1">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="B12" s="10">
+        <v>2</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="10">
+        <v>10</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10">
+        <v>10</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="10">
+        <v>3.1</v>
+      </c>
+      <c r="B13" s="10">
+        <v>2</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="10">
+        <v>10</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" s="8" customFormat="1">
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12">
-        <v>2.1</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" t="s">
+    <row r="14" spans="1:11" ht="28">
+      <c r="A14" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B14" s="10">
+        <v>2</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="10">
+        <v>10</v>
+      </c>
+      <c r="I14" s="10">
+        <v>6</v>
+      </c>
+      <c r="J14" s="10">
+        <v>6</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="10">
+        <v>2.4</v>
+      </c>
+      <c r="B15" s="10">
+        <v>2</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H12">
+      <c r="H15" s="10">
         <v>10</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="I15" s="10">
+        <v>12</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13">
-        <v>3.1</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" t="s">
+    <row r="16" spans="1:11">
+      <c r="A16" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H13">
+      <c r="H16" s="10">
+        <v>8</v>
+      </c>
+      <c r="I16" s="10">
         <v>10</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="J16" s="10">
+        <v>10</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="10">
+        <v>2.6</v>
+      </c>
+      <c r="B17" s="10">
+        <v>2</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="10">
+        <v>8</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28">
-      <c r="A14">
+    <row r="18" spans="1:11" ht="42">
+      <c r="A18" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="B18" s="10">
+        <v>2</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="10">
+        <v>4</v>
+      </c>
+      <c r="I18" s="10">
+        <v>2</v>
+      </c>
+      <c r="J18" s="10">
+        <v>2</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="10">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="B19" s="10">
+        <v>2</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="10">
+        <v>10</v>
+      </c>
+      <c r="I19" s="10">
+        <v>6</v>
+      </c>
+      <c r="J19" s="10">
+        <v>6</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="28">
+      <c r="A20" s="10">
+        <v>2.7</v>
+      </c>
+      <c r="B20" s="10">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10">
+        <v>6</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10">
+        <v>4</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="28">
+      <c r="A21" s="10">
+        <v>2.8</v>
+      </c>
+      <c r="B21" s="10">
+        <v>2</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="10">
+        <v>10</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10">
+        <v>4</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" s="7" customFormat="1">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="1:11" ht="28">
+      <c r="A24" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H14">
+      <c r="H24" s="10">
+        <v>12</v>
+      </c>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="42">
+      <c r="A25" s="10">
+        <v>4.2</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="10">
+        <v>18</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="10">
+        <v>4.3</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="10">
         <v>10</v>
       </c>
-      <c r="I14">
-        <v>6</v>
-      </c>
-      <c r="J14">
-        <v>6</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15">
-        <v>2.4</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15">
-        <v>10</v>
-      </c>
-      <c r="I15">
-        <v>12</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16">
-        <v>2.5</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16">
-        <v>8</v>
-      </c>
-      <c r="I16">
-        <v>10</v>
-      </c>
-      <c r="J16">
-        <v>10</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17">
-        <v>2.6</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="42">
-      <c r="A18">
-        <v>1.4</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18">
-        <v>4</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <v>2</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19">
-        <v>10</v>
-      </c>
-      <c r="I19">
-        <v>6</v>
-      </c>
-      <c r="J19">
-        <v>6</v>
-      </c>
-      <c r="K19" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="28">
-      <c r="A20">
-        <v>2.7</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20">
-        <v>6</v>
-      </c>
-      <c r="J20">
-        <v>4</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="28">
-      <c r="A21">
-        <v>2.8</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21">
-        <v>10</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="K22" s="10"/>
-    </row>
-    <row r="23" spans="1:11" s="8" customFormat="1">
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" ht="28">
-      <c r="A24">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24">
-        <v>12</v>
-      </c>
-      <c r="K24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="42">
-      <c r="A25">
-        <v>4.2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25">
-        <v>18</v>
-      </c>
-      <c r="K25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26">
-        <v>4.3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26">
-        <v>10</v>
-      </c>
-      <c r="K26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="C27" t="s">
-        <v>68</v>
-      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
updated scrum, and contact has now a to string method
</commit_message>
<xml_diff>
--- a/doc/scrum_green.xlsx
+++ b/doc/scrum_green.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -121,27 +121,12 @@
     <t>Create the Mainview of the Application in which the different views are displayed and a ViewManager</t>
   </si>
   <si>
-    <t>Data Model</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
     <t>Test the current Application on Errors</t>
   </si>
   <si>
-    <t>Design the Data Model for the Persistent Storage</t>
-  </si>
-  <si>
-    <t>Data Access</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>Create the Database Access Component, implementing the DataAccess Interface</t>
-  </si>
-  <si>
     <t>DataAccess</t>
   </si>
   <si>
@@ -251,6 +236,12 @@
   </si>
   <si>
     <t xml:space="preserve">Medication Settings View </t>
+  </si>
+  <si>
+    <t>Pseudo Persistent Storage</t>
+  </si>
+  <si>
+    <t>Allow acutal Data be viewed by Patient and Staff</t>
   </si>
 </sst>
 </file>
@@ -362,8 +353,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -468,7 +473,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="87">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -505,6 +510,13 @@
     <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -541,6 +553,13 @@
     <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -898,10 +917,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -918,7 +937,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
@@ -938,7 +957,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H4" t="s">
         <v>8</v>
@@ -964,10 +983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1040,7 +1059,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>5</v>
@@ -1053,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28">
@@ -1067,13 +1086,13 @@
         <v>27</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>5</v>
@@ -1086,7 +1105,7 @@
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1097,16 +1116,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>5</v>
@@ -1119,7 +1138,7 @@
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="42">
@@ -1130,16 +1149,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>5</v>
@@ -1154,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="28">
@@ -1171,7 +1190,7 @@
         <v>29</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>24</v>
@@ -1189,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="42">
@@ -1206,7 +1225,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>25</v>
@@ -1224,7 +1243,7 @@
         <v>6</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1287,14 +1306,14 @@
         <v>2</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>5</v>
@@ -1307,7 +1326,7 @@
         <v>10</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1318,14 +1337,14 @@
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>5</v>
@@ -1336,7 +1355,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="28">
@@ -1347,13 +1366,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>25</v>
@@ -1371,7 +1390,7 @@
         <v>6</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1382,14 +1401,14 @@
         <v>2</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>5</v>
@@ -1402,7 +1421,7 @@
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1413,13 +1432,13 @@
         <v>2</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>24</v>
@@ -1437,7 +1456,7 @@
         <v>10</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1448,16 +1467,16 @@
         <v>2</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>5</v>
@@ -1468,7 +1487,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="42">
@@ -1479,16 +1498,16 @@
         <v>2</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>5</v>
@@ -1503,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1514,13 +1533,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>25</v>
@@ -1538,7 +1557,7 @@
         <v>6</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28">
@@ -1549,13 +1568,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>24</v>
@@ -1569,7 +1588,7 @@
         <v>4</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="28">
@@ -1580,13 +1599,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>24</v>
@@ -1602,7 +1621,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1631,101 +1650,185 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
     </row>
-    <row r="24" spans="1:11" ht="28">
+    <row r="24" spans="1:11">
       <c r="A24" s="10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B24" s="10"/>
+      <c r="B24" s="10">
+        <v>3</v>
+      </c>
       <c r="C24" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="G24" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
-      <c r="K24" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="42">
+      <c r="K24" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="10">
         <v>4.2</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="10">
+        <v>3</v>
+      </c>
       <c r="C25" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>39</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D25" s="11"/>
       <c r="E25" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="10"/>
+        <v>60</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="G25" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H25" s="10">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
-      <c r="K25" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="K25" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28">
       <c r="A26" s="10">
         <v>4.3</v>
       </c>
-      <c r="B26" s="10"/>
+      <c r="B26" s="10">
+        <v>3</v>
+      </c>
       <c r="C26" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="G26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="10">
+        <v>8</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="10">
+        <v>3.1</v>
+      </c>
+      <c r="B27" s="10">
+        <v>3</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H27" s="10">
         <v>10</v>
       </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="K27" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="10">
+        <v>2.4</v>
+      </c>
+      <c r="B28" s="10">
+        <v>3</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="10">
+        <v>10</v>
+      </c>
+      <c r="I28" s="10">
+        <v>12</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="10">
+        <v>2.6</v>
+      </c>
+      <c r="B29" s="10">
+        <v>3</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="10">
+        <v>8</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>